<commit_message>
task 4, fixed normal distribution
</commit_message>
<xml_diff>
--- a/report/figures/task4/task4_tables.xlsx
+++ b/report/figures/task4/task4_tables.xlsx
@@ -525,31 +525,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>23.83682606297958</v>
+        <v>23.6125159492159</v>
       </c>
       <c r="C3" t="n">
-        <v>24.17757318652426</v>
+        <v>24.22894706844462</v>
       </c>
       <c r="D3" t="n">
-        <v>24.3592242172277</v>
+        <v>24.35516669106373</v>
       </c>
       <c r="E3" t="n">
-        <v>24.73779974364598</v>
+        <v>24.79639007135757</v>
       </c>
       <c r="F3" t="n">
-        <v>25</v>
+        <v>25.01058790125472</v>
       </c>
       <c r="G3" t="n">
-        <v>25.26220025635402</v>
+        <v>25.31578976705599</v>
       </c>
       <c r="H3" t="n">
-        <v>25.6407757827723</v>
+        <v>25.60961652558548</v>
       </c>
       <c r="I3" t="n">
-        <v>25.82242681347574</v>
+        <v>25.97094883707175</v>
       </c>
       <c r="J3" t="n">
-        <v>26.16317393702042</v>
+        <v>26.06482742811744</v>
       </c>
     </row>
     <row r="4">
@@ -559,31 +559,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.2243101137636785</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.05137388192035885</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.004057526163968816</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.05859032771158823</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.01058790125471987</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.05358951070197193</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>0.03115925718682178</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>0.1485220235960156</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>0.09834650890298491</v>
       </c>
     </row>
   </sheetData>
@@ -696,28 +696,28 @@
         <v>21</v>
       </c>
       <c r="C3" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D3" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E3" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G3" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H3" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="I3" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J3" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
@@ -730,28 +730,28 @@
         <v>2.836826062979579</v>
       </c>
       <c r="C4" t="n">
-        <v>11.17757318652426</v>
+        <v>4.177573186524263</v>
       </c>
       <c r="D4" t="n">
-        <v>8.359224217227698</v>
+        <v>5.359224217227698</v>
       </c>
       <c r="E4" t="n">
-        <v>3.737799743645979</v>
+        <v>2.737799743645979</v>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>2.737799743645979</v>
+        <v>0.7377997436459793</v>
       </c>
       <c r="H4" t="n">
-        <v>5.359224217227698</v>
+        <v>0.6407757827723017</v>
       </c>
       <c r="I4" t="n">
-        <v>6.177573186524263</v>
+        <v>4.177573186524263</v>
       </c>
       <c r="J4" t="n">
-        <v>9.836826062979579</v>
+        <v>6.836826062979579</v>
       </c>
     </row>
   </sheetData>
@@ -861,28 +861,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" t="n">
         <v>22</v>
       </c>
       <c r="F3" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H3" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I3" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" t="n">
         <v>38</v>
@@ -895,28 +895,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10.83682606297958</v>
+        <v>7.836826062979579</v>
       </c>
       <c r="C4" t="n">
-        <v>7.177573186524263</v>
+        <v>6.177573186524263</v>
       </c>
       <c r="D4" t="n">
-        <v>5.359224217227698</v>
+        <v>6.359224217227698</v>
       </c>
       <c r="E4" t="n">
         <v>2.737799743645979</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>1.737799743645979</v>
+        <v>2.737799743645979</v>
       </c>
       <c r="H4" t="n">
-        <v>5.359224217227698</v>
+        <v>6.359224217227698</v>
       </c>
       <c r="I4" t="n">
-        <v>8.177573186524263</v>
+        <v>7.177573186524263</v>
       </c>
       <c r="J4" t="n">
         <v>11.83682606297958</v>
@@ -1029,31 +1029,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.966401171300768</v>
+        <v>0.3530271770614896</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6395144029315324</v>
+        <v>0.08317540839287309</v>
       </c>
       <c r="D3" t="n">
-        <v>4.696140665390977</v>
+        <v>1.895093424053536</v>
       </c>
       <c r="E3" t="n">
-        <v>5.941669618816078</v>
+        <v>5.182297750219801</v>
       </c>
       <c r="F3" t="n">
-        <v>7.653053300287278</v>
+        <v>20.44251913370648</v>
       </c>
       <c r="G3" t="n">
-        <v>22.6016968138163</v>
+        <v>36.2338528758555</v>
       </c>
       <c r="H3" t="n">
-        <v>58.95783483648439</v>
+        <v>45.38043345149831</v>
       </c>
       <c r="I3" t="n">
-        <v>87.81273788991962</v>
+        <v>59.04172972873226</v>
       </c>
       <c r="J3" t="n">
-        <v>60.59265250332992</v>
+        <v>66.69359476997204</v>
       </c>
     </row>
     <row r="4">
@@ -1063,31 +1063,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>21.87042489167881</v>
+        <v>23.48379888591809</v>
       </c>
       <c r="C4" t="n">
-        <v>23.53805878359273</v>
+        <v>24.09439777813139</v>
       </c>
       <c r="D4" t="n">
-        <v>19.66308355183672</v>
+        <v>22.46413079317416</v>
       </c>
       <c r="E4" t="n">
-        <v>18.7961301248299</v>
+        <v>19.55550199342618</v>
       </c>
       <c r="F4" t="n">
-        <v>17.34694669971272</v>
+        <v>4.557480866293524</v>
       </c>
       <c r="G4" t="n">
-        <v>2.660503442537724</v>
+        <v>10.97165261950148</v>
       </c>
       <c r="H4" t="n">
-        <v>33.31705905371209</v>
+        <v>19.739657668726</v>
       </c>
       <c r="I4" t="n">
-        <v>61.99031107644388</v>
+        <v>33.21930291525653</v>
       </c>
       <c r="J4" t="n">
-        <v>34.4294785663095</v>
+        <v>40.53042083295162</v>
       </c>
     </row>
   </sheetData>
@@ -1197,31 +1197,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5298212518527636</v>
+        <v>0.1095801702055237</v>
       </c>
       <c r="C3" t="n">
-        <v>1.415473520225329</v>
+        <v>1.145873609188977</v>
       </c>
       <c r="D3" t="n">
-        <v>3.128020415978296</v>
+        <v>2.823217022293488</v>
       </c>
       <c r="E3" t="n">
-        <v>10.67143331273552</v>
+        <v>8.979461359037044</v>
       </c>
       <c r="F3" t="n">
-        <v>16.93297915564517</v>
+        <v>20.43130362617683</v>
       </c>
       <c r="G3" t="n">
-        <v>29.71993247422279</v>
+        <v>23.33631828311393</v>
       </c>
       <c r="H3" t="n">
-        <v>49.68249208703618</v>
+        <v>62.41232333411797</v>
       </c>
       <c r="I3" t="n">
-        <v>82.5274520402298</v>
+        <v>70.55005985866988</v>
       </c>
       <c r="J3" t="n">
-        <v>116.2333413941391</v>
+        <v>107.3466431768455</v>
       </c>
     </row>
     <row r="4">
@@ -1231,31 +1231,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>23.30700481112682</v>
+        <v>23.72724589277406</v>
       </c>
       <c r="C4" t="n">
-        <v>22.76209966629893</v>
+        <v>23.03169957733529</v>
       </c>
       <c r="D4" t="n">
-        <v>21.2312038012494</v>
+        <v>21.53600719493421</v>
       </c>
       <c r="E4" t="n">
-        <v>14.06636643091046</v>
+        <v>15.75833838460894</v>
       </c>
       <c r="F4" t="n">
-        <v>8.067020844354829</v>
+        <v>4.568696373823169</v>
       </c>
       <c r="G4" t="n">
-        <v>4.457732217868774</v>
+        <v>1.925881973240095</v>
       </c>
       <c r="H4" t="n">
-        <v>24.04171630426388</v>
+        <v>36.77154755134567</v>
       </c>
       <c r="I4" t="n">
-        <v>56.70502522675407</v>
+        <v>44.72763304519415</v>
       </c>
       <c r="J4" t="n">
-        <v>90.07016745711864</v>
+        <v>81.18346923982506</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
task4: added normal with n=10 and n=200
</commit_message>
<xml_diff>
--- a/report/figures/task4/task4_tables.xlsx
+++ b/report/figures/task4/task4_tables.xlsx
@@ -7,11 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Normal (Correct)" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Poisson n=10" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Poisson n=200" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Exponential n=10" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Exponential n=200" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Normal n=10" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Normal n=200" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Poisson n=10" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Poisson n=200" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Exponential n=10" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Exponential n=200" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -525,31 +526,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>23.6125159492159</v>
+        <v>23.72115090977198</v>
       </c>
       <c r="C3" t="n">
-        <v>24.22894706844462</v>
+        <v>24.11286926053632</v>
       </c>
       <c r="D3" t="n">
-        <v>24.35516669106373</v>
+        <v>24.27829104897748</v>
       </c>
       <c r="E3" t="n">
-        <v>24.79639007135757</v>
+        <v>24.81041113890068</v>
       </c>
       <c r="F3" t="n">
-        <v>25.01058790125472</v>
+        <v>24.90538370708719</v>
       </c>
       <c r="G3" t="n">
-        <v>25.31578976705599</v>
+        <v>25.32664334295132</v>
       </c>
       <c r="H3" t="n">
-        <v>25.60961652558548</v>
+        <v>25.76233998830304</v>
       </c>
       <c r="I3" t="n">
-        <v>25.97094883707175</v>
+        <v>25.56985130617119</v>
       </c>
       <c r="J3" t="n">
-        <v>26.06482742811744</v>
+        <v>25.55307652794273</v>
       </c>
     </row>
     <row r="4">
@@ -559,31 +560,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2243101137636785</v>
+        <v>0.1156751532075972</v>
       </c>
       <c r="C4" t="n">
-        <v>0.05137388192035885</v>
+        <v>0.0647039259879385</v>
       </c>
       <c r="D4" t="n">
-        <v>0.004057526163968816</v>
+        <v>0.08093316825021546</v>
       </c>
       <c r="E4" t="n">
-        <v>0.05859032771158823</v>
+        <v>0.07261139525470028</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01058790125471987</v>
+        <v>0.09461629291281426</v>
       </c>
       <c r="G4" t="n">
-        <v>0.05358951070197193</v>
+        <v>0.06444308659730424</v>
       </c>
       <c r="H4" t="n">
-        <v>0.03115925718682178</v>
+        <v>0.1215642055307349</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1485220235960156</v>
+        <v>0.2525755073045488</v>
       </c>
       <c r="J4" t="n">
-        <v>0.09834650890298491</v>
+        <v>0.6100974090776887</v>
       </c>
     </row>
   </sheetData>
@@ -693,31 +694,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>21</v>
+        <v>23.94440780310197</v>
       </c>
       <c r="C3" t="n">
-        <v>20</v>
+        <v>24.13637732680318</v>
       </c>
       <c r="D3" t="n">
-        <v>19</v>
+        <v>24.32952681776699</v>
       </c>
       <c r="E3" t="n">
-        <v>22</v>
+        <v>24.70383043293115</v>
       </c>
       <c r="F3" t="n">
-        <v>25</v>
+        <v>24.98537011147862</v>
       </c>
       <c r="G3" t="n">
-        <v>26</v>
+        <v>25.2905742930021</v>
       </c>
       <c r="H3" t="n">
-        <v>25</v>
+        <v>25.62040023891179</v>
       </c>
       <c r="I3" t="n">
-        <v>30</v>
+        <v>25.79165086729704</v>
       </c>
       <c r="J3" t="n">
-        <v>33</v>
+        <v>26.01469569035935</v>
       </c>
     </row>
     <row r="4">
@@ -727,31 +728,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2.836826062979579</v>
+        <v>0.107581740122388</v>
       </c>
       <c r="C4" t="n">
-        <v>4.177573186524263</v>
+        <v>0.04119585972108553</v>
       </c>
       <c r="D4" t="n">
-        <v>5.359224217227698</v>
+        <v>0.0296973994607086</v>
       </c>
       <c r="E4" t="n">
-        <v>2.737799743645979</v>
+        <v>0.03396931071483067</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.0146298885213767</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7377997436459793</v>
+        <v>0.02837403664808136</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6407757827723017</v>
+        <v>0.02037554386051355</v>
       </c>
       <c r="I4" t="n">
-        <v>4.177573186524263</v>
+        <v>0.0307759461786965</v>
       </c>
       <c r="J4" t="n">
-        <v>6.836826062979579</v>
+        <v>0.1484782466610746</v>
       </c>
     </row>
   </sheetData>
@@ -861,31 +862,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E3" t="n">
         <v>22</v>
       </c>
       <c r="F3" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G3" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H3" t="n">
         <v>32</v>
       </c>
       <c r="I3" t="n">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="J3" t="n">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -895,31 +896,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7.836826062979579</v>
+        <v>6.836826062979579</v>
       </c>
       <c r="C4" t="n">
-        <v>6.177573186524263</v>
+        <v>5.177573186524263</v>
       </c>
       <c r="D4" t="n">
-        <v>6.359224217227698</v>
+        <v>11.3592242172277</v>
       </c>
       <c r="E4" t="n">
         <v>2.737799743645979</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>2.737799743645979</v>
+        <v>0.2622002563540207</v>
       </c>
       <c r="H4" t="n">
         <v>6.359224217227698</v>
       </c>
       <c r="I4" t="n">
-        <v>7.177573186524263</v>
+        <v>0.1775731865242633</v>
       </c>
       <c r="J4" t="n">
-        <v>11.83682606297958</v>
+        <v>5.836826062979579</v>
       </c>
     </row>
   </sheetData>
@@ -1029,31 +1030,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3530271770614896</v>
+        <v>13</v>
       </c>
       <c r="C3" t="n">
-        <v>0.08317540839287309</v>
+        <v>17</v>
       </c>
       <c r="D3" t="n">
-        <v>1.895093424053536</v>
+        <v>19</v>
       </c>
       <c r="E3" t="n">
-        <v>5.182297750219801</v>
+        <v>22</v>
       </c>
       <c r="F3" t="n">
-        <v>20.44251913370648</v>
+        <v>25</v>
       </c>
       <c r="G3" t="n">
-        <v>36.2338528758555</v>
+        <v>28</v>
       </c>
       <c r="H3" t="n">
-        <v>45.38043345149831</v>
+        <v>30</v>
       </c>
       <c r="I3" t="n">
-        <v>59.04172972873226</v>
+        <v>33</v>
       </c>
       <c r="J3" t="n">
-        <v>66.69359476997204</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4">
@@ -1063,31 +1064,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>23.48379888591809</v>
+        <v>10.83682606297958</v>
       </c>
       <c r="C4" t="n">
-        <v>24.09439777813139</v>
+        <v>7.177573186524263</v>
       </c>
       <c r="D4" t="n">
-        <v>22.46413079317416</v>
+        <v>5.359224217227698</v>
       </c>
       <c r="E4" t="n">
-        <v>19.55550199342618</v>
+        <v>2.737799743645979</v>
       </c>
       <c r="F4" t="n">
-        <v>4.557480866293524</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>10.97165261950148</v>
+        <v>2.737799743645979</v>
       </c>
       <c r="H4" t="n">
-        <v>19.739657668726</v>
+        <v>4.359224217227698</v>
       </c>
       <c r="I4" t="n">
-        <v>33.21930291525653</v>
+        <v>7.177573186524263</v>
       </c>
       <c r="J4" t="n">
-        <v>40.53042083295162</v>
+        <v>10.83682606297958</v>
       </c>
     </row>
   </sheetData>
@@ -1197,31 +1198,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1095801702055237</v>
+        <v>3.319333386610535</v>
       </c>
       <c r="C3" t="n">
-        <v>1.145873609188977</v>
+        <v>6.645241065934061</v>
       </c>
       <c r="D3" t="n">
-        <v>2.823217022293488</v>
+        <v>2.600606557051416</v>
       </c>
       <c r="E3" t="n">
-        <v>8.979461359037044</v>
+        <v>14.21955058144925</v>
       </c>
       <c r="F3" t="n">
-        <v>20.43130362617683</v>
+        <v>10.04913025526181</v>
       </c>
       <c r="G3" t="n">
-        <v>23.33631828311393</v>
+        <v>22.97451111096569</v>
       </c>
       <c r="H3" t="n">
-        <v>62.41232333411797</v>
+        <v>56.56680204231566</v>
       </c>
       <c r="I3" t="n">
-        <v>70.55005985866988</v>
+        <v>63.57232107716722</v>
       </c>
       <c r="J3" t="n">
-        <v>107.3466431768455</v>
+        <v>94.18889952448856</v>
       </c>
     </row>
     <row r="4">
@@ -1231,31 +1232,199 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>23.72724589277406</v>
+        <v>20.51749267636905</v>
       </c>
       <c r="C4" t="n">
-        <v>23.03169957733529</v>
+        <v>17.5323321205902</v>
       </c>
       <c r="D4" t="n">
-        <v>21.53600719493421</v>
+        <v>21.75861766017628</v>
       </c>
       <c r="E4" t="n">
-        <v>15.75833838460894</v>
+        <v>10.51824916219673</v>
       </c>
       <c r="F4" t="n">
-        <v>4.568696373823169</v>
+        <v>14.95086974473819</v>
       </c>
       <c r="G4" t="n">
-        <v>1.925881973240095</v>
+        <v>2.287689145388335</v>
       </c>
       <c r="H4" t="n">
-        <v>36.77154755134567</v>
+        <v>30.92602625954336</v>
       </c>
       <c r="I4" t="n">
-        <v>44.72763304519415</v>
+        <v>37.74989426369149</v>
       </c>
       <c r="J4" t="n">
-        <v>81.18346923982506</v>
+        <v>68.02572558746814</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>0.70</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>0.90</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>0.95</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>0.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Estimated (Q_hat)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>23.83682606297958</v>
+      </c>
+      <c r="C2" t="n">
+        <v>24.17757318652426</v>
+      </c>
+      <c r="D2" t="n">
+        <v>24.3592242172277</v>
+      </c>
+      <c r="E2" t="n">
+        <v>24.73779974364598</v>
+      </c>
+      <c r="F2" t="n">
+        <v>25</v>
+      </c>
+      <c r="G2" t="n">
+        <v>25.26220025635402</v>
+      </c>
+      <c r="H2" t="n">
+        <v>25.6407757827723</v>
+      </c>
+      <c r="I2" t="n">
+        <v>25.82242681347574</v>
+      </c>
+      <c r="J2" t="n">
+        <v>26.16317393702042</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>True (Q_star)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.3329494521512377</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.107283663289776</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.420319426982381</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10.94422683552016</v>
+      </c>
+      <c r="F3" t="n">
+        <v>16.11517693407245</v>
+      </c>
+      <c r="G3" t="n">
+        <v>29.71625107167191</v>
+      </c>
+      <c r="H3" t="n">
+        <v>62.36024255845448</v>
+      </c>
+      <c r="I3" t="n">
+        <v>70.76272145457925</v>
+      </c>
+      <c r="J3" t="n">
+        <v>117.2865506316603</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Absolute Error</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>23.50387661082834</v>
+      </c>
+      <c r="C4" t="n">
+        <v>23.07028952323449</v>
+      </c>
+      <c r="D4" t="n">
+        <v>22.93890479024532</v>
+      </c>
+      <c r="E4" t="n">
+        <v>13.79357290812582</v>
+      </c>
+      <c r="F4" t="n">
+        <v>8.884823065927552</v>
+      </c>
+      <c r="G4" t="n">
+        <v>4.454050815317885</v>
+      </c>
+      <c r="H4" t="n">
+        <v>36.71946677568218</v>
+      </c>
+      <c r="I4" t="n">
+        <v>44.94029464110351</v>
+      </c>
+      <c r="J4" t="n">
+        <v>91.12337669463992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>